<commit_message>
Commiting Contacts page Testcases
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ashishProject\freecrmproject\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C56924-AB86-46A3-B728-A95EB8ECAB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7B3FB7-0168-43A3-8300-4531CC147121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="3240" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ContactInformation" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>Title</t>
   </si>
@@ -55,6 +55,36 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Mrs.</t>
+  </si>
+  <si>
+    <t>Anisha</t>
+  </si>
+  <si>
+    <t>Snehal</t>
+  </si>
+  <si>
+    <t>Suffix</t>
+  </si>
+  <si>
+    <t>Esq.</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>File Path</t>
+  </si>
+  <si>
+    <t>D:\ashishProject\freecrmproject\TestData\image1.jfif</t>
+  </si>
+  <si>
+    <t>D:\ashishProject\freecrmproject\TestData\image2.jfif</t>
   </si>
 </sst>
 </file>
@@ -405,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -417,10 +447,12 @@
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="24.88671875" style="2"/>
+    <col min="5" max="5" width="10.77734375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="51.6640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="24.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -434,10 +466,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -451,6 +489,58 @@
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>